<commit_message>
Dokumentáció frissítés 4 - configok
</commit_message>
<xml_diff>
--- a/doksi_táblázat.xlsx
+++ b/doksi_táblázat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gergő\Documents\GitHub\Project-Atlas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85014D12-56E0-4167-9A7A-F94FF44BBF60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0186E595-8AC9-4F3E-8EA6-D35386DBD7A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="102">
   <si>
     <t>R-FL1</t>
   </si>
@@ -292,30 +292,9 @@
     <t>-</t>
   </si>
   <si>
-    <t>Internet</t>
-  </si>
-  <si>
-    <t>BR-WR</t>
-  </si>
-  <si>
-    <t>BR-WR, WR-FL1</t>
-  </si>
-  <si>
-    <t>BR-WR, R-FL1</t>
-  </si>
-  <si>
-    <t>192.168.50.1 /24</t>
-  </si>
-  <si>
-    <t>192.168.50.2 /24</t>
-  </si>
-  <si>
     <t>Eth1</t>
   </si>
   <si>
-    <t>Eth2</t>
-  </si>
-  <si>
     <t>IP cím (WR=LAN)</t>
   </si>
   <si>
@@ -337,10 +316,22 @@
     <t>IP cím/LAN</t>
   </si>
   <si>
-    <t>Eth0/1</t>
-  </si>
-  <si>
-    <t>Eth1/1</t>
+    <t>R-WR</t>
+  </si>
+  <si>
+    <t>192.168.50.2 /30</t>
+  </si>
+  <si>
+    <t>192.168.50.1 /30</t>
+  </si>
+  <si>
+    <t>192.168.5.2 /24</t>
+  </si>
+  <si>
+    <t>192.168.6.2 /24</t>
+  </si>
+  <si>
+    <t>192.168.7.2 /24</t>
   </si>
 </sst>
 </file>
@@ -372,7 +363,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -865,56 +856,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -963,7 +909,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
@@ -972,48 +939,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1330,10 +1262,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC31"/>
+  <dimension ref="A1:AC27"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1374,7 +1306,7 @@
         <v>67</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="F1" s="17"/>
       <c r="G1" s="18" t="s">
@@ -1421,17 +1353,17 @@
       </c>
     </row>
     <row r="2" spans="1:29" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="49" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="D2" s="50" t="s">
-        <v>93</v>
+      <c r="A2" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>97</v>
       </c>
       <c r="F2" s="31" t="s">
         <v>85</v>
@@ -1442,7 +1374,7 @@
       <c r="H2" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="K2" s="32" t="s">
+      <c r="K2" s="46" t="s">
         <v>0</v>
       </c>
       <c r="L2" s="4" t="s">
@@ -1454,7 +1386,7 @@
       <c r="N2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="P2" s="35" t="s">
+      <c r="P2" s="43" t="s">
         <v>4</v>
       </c>
       <c r="Q2" s="2" t="s">
@@ -1466,7 +1398,7 @@
       <c r="S2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="U2" s="35" t="s">
+      <c r="U2" s="43" t="s">
         <v>18</v>
       </c>
       <c r="V2" s="2" t="s">
@@ -1480,15 +1412,15 @@
       </c>
     </row>
     <row r="3" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="51"/>
-      <c r="B3" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>97</v>
+      <c r="A3" s="44"/>
+      <c r="B3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>90</v>
       </c>
       <c r="F3" s="30" t="s">
         <v>72</v>
@@ -1499,7 +1431,7 @@
       <c r="H3" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="K3" s="33"/>
+      <c r="K3" s="44"/>
       <c r="L3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1509,7 +1441,7 @@
       <c r="N3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="33"/>
+      <c r="P3" s="44"/>
       <c r="Q3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1519,7 +1451,7 @@
       <c r="S3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="U3" s="33"/>
+      <c r="U3" s="44"/>
       <c r="V3" s="1" t="s">
         <v>20</v>
       </c>
@@ -1531,15 +1463,15 @@
       </c>
     </row>
     <row r="4" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51"/>
-      <c r="B4" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>97</v>
+      <c r="A4" s="44"/>
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>92</v>
       </c>
       <c r="F4" s="28" t="s">
         <v>80</v>
@@ -1550,7 +1482,7 @@
       <c r="H4" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="K4" s="33"/>
+      <c r="K4" s="44"/>
       <c r="L4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1560,7 +1492,7 @@
       <c r="N4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="P4" s="33"/>
+      <c r="P4" s="44"/>
       <c r="Q4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1570,7 +1502,7 @@
       <c r="S4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="U4" s="33"/>
+      <c r="U4" s="44"/>
       <c r="V4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1594,17 +1526,15 @@
       </c>
     </row>
     <row r="5" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>99</v>
+      <c r="A5" s="45"/>
+      <c r="B5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>93</v>
       </c>
       <c r="F5" s="30" t="s">
         <v>80</v>
@@ -1615,21 +1545,19 @@
       <c r="H5" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="K5" s="34"/>
+      <c r="K5" s="45"/>
       <c r="L5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="M5" s="3"/>
       <c r="N5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="P5" s="34"/>
+      <c r="P5" s="45"/>
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
       <c r="S5" s="9"/>
-      <c r="U5" s="33"/>
+      <c r="U5" s="44"/>
       <c r="V5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1639,7 +1567,7 @@
       <c r="X5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="Z5" s="35" t="s">
+      <c r="Z5" s="43" t="s">
         <v>47</v>
       </c>
       <c r="AA5" s="2" t="s">
@@ -1653,17 +1581,17 @@
       </c>
     </row>
     <row r="6" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="42" t="s">
+      <c r="A6" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C6" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="43" t="s">
-        <v>100</v>
+      <c r="C6" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>99</v>
       </c>
       <c r="F6" s="31" t="s">
         <v>73</v>
@@ -1698,11 +1626,11 @@
       <c r="S6" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="U6" s="34"/>
+      <c r="U6" s="45"/>
       <c r="V6" s="5"/>
       <c r="W6" s="5"/>
       <c r="X6" s="16"/>
-      <c r="Z6" s="34"/>
+      <c r="Z6" s="45"/>
       <c r="AA6" s="3" t="s">
         <v>48</v>
       </c>
@@ -1714,16 +1642,18 @@
       </c>
     </row>
     <row r="7" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="52" t="s">
-        <v>89</v>
-      </c>
-      <c r="B7" s="53" t="s">
-        <v>103</v>
-      </c>
-      <c r="C7" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="7"/>
+      <c r="A7" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>100</v>
+      </c>
       <c r="F7" s="29" t="s">
         <v>73</v>
       </c>
@@ -1783,21 +1713,25 @@
       </c>
     </row>
     <row r="8" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="54"/>
-      <c r="B8" s="55" t="s">
-        <v>104</v>
-      </c>
-      <c r="C8" s="55" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="15"/>
-      <c r="F8" s="41" t="s">
+      <c r="A8" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="F8" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="G8" s="42" t="s">
+      <c r="G8" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="H8" s="43" t="s">
+      <c r="H8" s="38" t="s">
         <v>77</v>
       </c>
       <c r="K8" s="6" t="s">
@@ -1850,12 +1784,12 @@
       </c>
     </row>
     <row r="9" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F9" s="44" t="s">
-        <v>98</v>
-      </c>
-      <c r="G9" s="45"/>
-      <c r="H9" s="46" t="s">
-        <v>101</v>
+      <c r="F9" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="G9" s="40"/>
+      <c r="H9" s="41" t="s">
+        <v>94</v>
       </c>
       <c r="K9" s="13" t="s">
         <v>56</v>
@@ -1909,74 +1843,28 @@
       </c>
     </row>
     <row r="11" spans="1:29" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K22" s="36"/>
-      <c r="L22" s="36"/>
-      <c r="M22" s="36"/>
-      <c r="N22" s="36"/>
-    </row>
-    <row r="23" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K23" s="37"/>
-      <c r="L23" s="36"/>
-      <c r="M23" s="36"/>
-      <c r="N23" s="36"/>
-    </row>
-    <row r="24" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K24" s="37"/>
-      <c r="L24" s="36"/>
-      <c r="M24" s="36"/>
-      <c r="N24" s="36"/>
-    </row>
-    <row r="25" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K25" s="37"/>
-      <c r="L25" s="36"/>
-      <c r="M25" s="36"/>
-      <c r="N25" s="36"/>
-    </row>
-    <row r="26" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K26" s="37"/>
-      <c r="L26" s="36"/>
-      <c r="M26" s="36"/>
-      <c r="N26" s="36"/>
-    </row>
-    <row r="27" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K27" s="37"/>
-      <c r="L27" s="36"/>
-      <c r="M27" s="36"/>
-      <c r="N27" s="36"/>
-    </row>
-    <row r="28" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K28" s="36"/>
-      <c r="L28" s="36"/>
-      <c r="M28" s="36"/>
-      <c r="N28" s="36"/>
-    </row>
-    <row r="29" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K29" s="36"/>
-      <c r="L29" s="36"/>
-      <c r="M29" s="36"/>
-      <c r="N29" s="36"/>
-    </row>
-    <row r="30" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K30" s="36"/>
-      <c r="L30" s="36"/>
-      <c r="M30" s="36"/>
-      <c r="N30" s="36"/>
-    </row>
-    <row r="31" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K31" s="36"/>
-      <c r="L31" s="36"/>
-      <c r="M31" s="36"/>
-      <c r="N31" s="36"/>
+    <row r="23" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K23" s="33"/>
+    </row>
+    <row r="24" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K24" s="33"/>
+    </row>
+    <row r="25" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K25" s="33"/>
+    </row>
+    <row r="26" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K26" s="33"/>
+    </row>
+    <row r="27" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K27" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="5">
+    <mergeCell ref="Z5:Z6"/>
+    <mergeCell ref="A2:A5"/>
     <mergeCell ref="U2:U6"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A7:A8"/>
     <mergeCell ref="K2:K5"/>
     <mergeCell ref="P2:P5"/>
-    <mergeCell ref="Z5:Z6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1986,10 +1874,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25BB4C48-F5D0-46DF-BAA6-65E9341EA299}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2000,7 +1888,7 @@
     <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>68</v>
       </c>
@@ -2011,12 +1899,11 @@
         <v>67</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="E1" s="36"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="46" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -2028,10 +1915,9 @@
       <c r="D2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="36"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="44"/>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
@@ -2041,10 +1927,9 @@
       <c r="D3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="36"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="33"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="44"/>
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
@@ -2054,23 +1939,21 @@
       <c r="D4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="36"/>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="34"/>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="45"/>
       <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="E5" s="36"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="43" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -2082,10 +1965,9 @@
       <c r="D6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="36"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="33"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="44"/>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -2095,10 +1977,9 @@
       <c r="D7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="36"/>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="33"/>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="44"/>
       <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
@@ -2108,10 +1989,9 @@
       <c r="D8" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="36"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="43" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -2123,10 +2003,9 @@
       <c r="D9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="36"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="44"/>
       <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
@@ -2136,10 +2015,9 @@
       <c r="D10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="36"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="33"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="44"/>
       <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
@@ -2149,361 +2027,341 @@
       <c r="D11" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="36"/>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="33"/>
-      <c r="B12" s="1" t="s">
+    </row>
+    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="44"/>
+      <c r="B12" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="36"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="35" t="s">
-        <v>47</v>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="43" t="s">
+        <v>96</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="44"/>
+      <c r="B14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="44"/>
+      <c r="B15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="45"/>
+      <c r="B16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D17" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="36"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="34"/>
-      <c r="B14" s="3" t="s">
+    </row>
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="45"/>
+      <c r="B18" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D18" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E14" s="36"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="E15" s="36"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="33"/>
-      <c r="B16" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="C19" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="E16" s="36"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="40"/>
-      <c r="B17" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C17" s="4" t="s">
+      <c r="B20" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="E17" s="36"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1" t="s">
+      <c r="B21" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="E18" s="36"/>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="38" t="s">
-        <v>88</v>
-      </c>
-      <c r="C19" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="39" t="s">
-        <v>100</v>
-      </c>
-      <c r="E19" s="36"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
+      <c r="C21" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D22" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="36"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="26" t="s">
         <v>35</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E21" s="36"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="E22" s="36"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="26" t="s">
-        <v>36</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" s="36"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="36"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D27" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="36"/>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="27" t="s">
+    </row>
+    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B28" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D28" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E26" s="36"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D29" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="E27" s="36"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="29" t="s">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="29" t="s">
         <v>56</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E28" s="36"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E29" s="36"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="29" t="s">
-        <v>58</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E30" s="36"/>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="30" t="s">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B33" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D33" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E31" s="36"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="31" t="s">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B34" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C34" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D34" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="E32" s="36"/>
-    </row>
-    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="41" t="s">
+    </row>
+    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="42" t="s">
+      <c r="B35" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="C33" s="42" t="s">
+      <c r="C35" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="D33" s="43" t="s">
+      <c r="D35" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="E33" s="36"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="52" t="s">
-        <v>89</v>
-      </c>
-      <c r="B34" s="53" t="s">
-        <v>103</v>
-      </c>
-      <c r="C34" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="D34" s="7"/>
-    </row>
-    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="54"/>
-      <c r="B35" s="55" t="s">
-        <v>104</v>
-      </c>
-      <c r="C35" s="55" t="s">
-        <v>12</v>
-      </c>
-      <c r="D35" s="15"/>
-    </row>
-    <row r="36" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="5">
+    <mergeCell ref="A13:A16"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A17:A18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>